<commit_message>
Updated the lab instructions
</commit_message>
<xml_diff>
--- a/LabStarters/Lab08/Lab8Rubric-CIS195.xlsx
+++ b/LabStarters/Lab08/Lab8Rubric-CIS195.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CIS195-CourseMaterials/LabStarters/Lab08/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CIS195-CourseMaterials\LabStarters\Lab08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DB4691-980F-2941-AD35-56A4A7123A56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A9D9B77-4CB0-4A1E-B808-7F6A48051AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="20920" windowHeight="22120" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="3456" yWindow="3456" windowWidth="23040" windowHeight="12204" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Student Scores" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Requirements:</t>
   </si>
@@ -43,18 +54,9 @@
     <t>Syntax and Style are correct</t>
   </si>
   <si>
-    <t>Part 2: Calendar for a month</t>
-  </si>
-  <si>
     <t>Lab 8, Multimedia</t>
   </si>
   <si>
-    <t>Part 1</t>
-  </si>
-  <si>
-    <t>Fall term, 2019, there was no part 2</t>
-  </si>
-  <si>
     <t>&lt;audio&gt; elemement</t>
   </si>
   <si>
@@ -65,9 +67,6 @@
   </si>
   <si>
     <t>The page conatins one each:</t>
-  </si>
-  <si>
-    <t>Subtotal</t>
   </si>
 </sst>
 </file>
@@ -473,198 +472,124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="24.3984375" customWidth="1"/>
+    <col min="2" max="2" width="7.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="E5">
         <v>10</v>
       </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="E6">
         <v>15</v>
       </c>
-      <c r="F6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-      <c r="E7">
         <v>20</v>
       </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="4">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <f>SUM(B4:B8)</f>
-        <v>20</v>
-      </c>
-      <c r="C9" s="3">
-        <f>SUM(C4:C8)</f>
-        <v>20</v>
-      </c>
-      <c r="E9" s="5">
-        <f>SUM(E4:E8)</f>
         <v>50</v>
       </c>
-      <c r="F9" s="5">
-        <f>SUM(F4:F8)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C9" s="3"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3">
-        <f>SUM(B13:B15)</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="3">
-        <f>SUM(C13:C15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="5">
-        <f>SUM(B9,B16)</f>
-        <v>20</v>
-      </c>
-      <c r="C17" s="5">
-        <f>SUM(C9,C16)</f>
-        <v>20</v>
-      </c>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <webPublishItems count="1">
+    <webPublishItem id="28190" divId="Lab8Rubric-CIS195_28190" sourceType="range" sourceRef="A1:B9" destinationFile="D:\Repos\CIS195-CourseMaterials\LabStarters\Lab08\Lab8Rubric-CIS195.htm"/>
+  </webPublishItems>
 </worksheet>
 </file>
 
@@ -672,23 +597,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView zoomScale="156" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="1" max="1" width="25.59765625" customWidth="1"/>
+    <col min="2" max="2" width="8.796875" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -696,14 +617,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -712,9 +633,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -723,9 +644,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -734,7 +655,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -745,7 +666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
@@ -758,95 +679,95 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>

</xml_diff>